<commit_message>
latest processed data after running the motilal_portfolio_change_engine
</commit_message>
<xml_diff>
--- a/mf-intelligence/data/processed/invesco/Invesco_India_Business_Cycle_Fund_Equity_Holdings_Comparison.xlsx
+++ b/mf-intelligence/data/processed/invesco/Invesco_India_Business_Cycle_Fund_Equity_Holdings_Comparison.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,35 +446,40 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Mutual Fund</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Jan_2026</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Dec_2025</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Oct_2025</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>MoM</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>QoQ</t>
         </is>
@@ -493,27 +498,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Transport Services</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>5.99</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>5.61</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>4.35</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.3799999999999999</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>1.640000000000001</v>
       </c>
     </row>
@@ -530,27 +540,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Banks</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>5.89</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>5.62</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>5.44</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.2699999999999996</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.4499999999999993</v>
       </c>
     </row>
@@ -567,27 +582,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Healthcare Services</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>5.63</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>4.52</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>4.99</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>1.11</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.6399999999999997</v>
       </c>
     </row>
@@ -604,27 +624,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Retailing</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>4.63</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>4.44</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>4.27</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>0.1899999999999995</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.3600000000000003</v>
       </c>
     </row>
@@ -641,27 +666,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Realty</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>4.59</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>3.41</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>4.09</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>1.18</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -678,27 +708,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Banks</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>4.54</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>3.98</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>3.03</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>0.5600000000000001</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>1.51</v>
       </c>
     </row>
@@ -715,27 +750,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Pharmaceuticals &amp; Biotechnology</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>4.43</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>4.54</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>5.03</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>-0.1100000000000003</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>-0.6000000000000005</v>
       </c>
     </row>
@@ -752,27 +792,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Adding</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>4.34</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>4.27</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>4.66</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>0.07000000000000028</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>-0.3200000000000003</v>
       </c>
     </row>
@@ -789,27 +834,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Retailing</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>4.34</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>4.63</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>4.72</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>-0.29</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>-0.3799999999999999</v>
       </c>
     </row>
@@ -826,27 +876,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Retailing</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>4.15</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>4.88</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>4.91</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>-0.7299999999999995</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>-0.7599999999999998</v>
       </c>
     </row>
@@ -863,27 +918,32 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Reducing</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>3.85</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>4</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>3.29</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>-0.1499999999999999</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>0.5600000000000001</v>
       </c>
     </row>
@@ -900,27 +960,32 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Industrial Manufacturing</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>Reducing</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>3.71</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>3.77</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>3.64</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>-0.06000000000000005</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>0.06999999999999984</v>
       </c>
     </row>
@@ -937,27 +1002,32 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Consumer Durables</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>3.59</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>3.78</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>3.62</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>-0.1899999999999999</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>-0.03000000000000025</v>
       </c>
     </row>
@@ -974,27 +1044,32 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>3.46</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>3.18</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>1.66</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>0.2799999999999998</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>1.8</v>
       </c>
     </row>
@@ -1011,27 +1086,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Commercial Services &amp; Supplies</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>Stable</t>
         </is>
-      </c>
-      <c r="E16" t="n">
-        <v>3.41</v>
       </c>
       <c r="F16" t="n">
         <v>3.41</v>
       </c>
       <c r="G16" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="H16" t="n">
         <v>3.99</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>0</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>-0.5800000000000001</v>
       </c>
     </row>
@@ -1048,27 +1128,32 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Capital Markets</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>3.23</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>2.87</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>2.96</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.3599999999999999</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.27</v>
       </c>
     </row>
@@ -1085,27 +1170,32 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Cement &amp; Cement Products</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>2.98</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>1.71</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>2.1</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>1.27</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.8799999999999999</v>
       </c>
     </row>
@@ -1122,27 +1212,32 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>IT - Software</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>2.72</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>2.91</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>3.28</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>-0.1899999999999999</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>-0.5599999999999996</v>
       </c>
     </row>
@@ -1159,27 +1254,32 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Healthcare Services</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>2.6</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>2.76</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>3.35</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>-0.1599999999999997</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>-0.75</v>
       </c>
     </row>
@@ -1196,27 +1296,32 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Healthcare Services</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>Adding</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>2.59</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>2.46</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>3.2</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>0.1299999999999999</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>-0.6100000000000003</v>
       </c>
     </row>
@@ -1233,29 +1338,34 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Banks</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>Fresh Entry</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>2.58</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>2.58</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
         <v>2.58</v>
       </c>
+      <c r="J22" t="n">
+        <v>2.58</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1270,27 +1380,32 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Healthcare Services</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>Adding</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>2.56</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>2.44</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>2.91</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>0.1200000000000001</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>-0.3500000000000001</v>
       </c>
     </row>
@@ -1307,27 +1422,32 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Capital Markets</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>Stable</t>
         </is>
-      </c>
-      <c r="E24" t="n">
-        <v>2.34</v>
       </c>
       <c r="F24" t="n">
         <v>2.34</v>
       </c>
       <c r="G24" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="H24" t="n">
         <v>2.58</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>0</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>-0.2400000000000002</v>
       </c>
     </row>
@@ -1344,27 +1464,32 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>IT - Software</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>1.74</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>1.8</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>1.77</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>-0.06000000000000005</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>-0.03000000000000003</v>
       </c>
     </row>
@@ -1381,27 +1506,32 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Pharmaceuticals &amp; Biotechnology</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>1.74</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>1.65</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>1.68</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>0.09000000000000008</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>0.06000000000000005</v>
       </c>
     </row>
@@ -1418,27 +1548,32 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Realty</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>1.71</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>1.88</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>2.14</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>-0.1699999999999999</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>-0.4300000000000002</v>
       </c>
     </row>
@@ -1455,29 +1590,34 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Realty</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>1.26</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1.31</v>
       </c>
       <c r="G28" t="n">
         <v>1.31</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.05000000000000004</v>
+        <v>1.31</v>
       </c>
       <c r="I28" t="n">
         <v>-0.05000000000000004</v>
       </c>
+      <c r="J28" t="n">
+        <v>-0.05000000000000004</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1492,27 +1632,32 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Electrical Equipment</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>Adding Consistently</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>1.06</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>0.93</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>1.03</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>0.13</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>0.03000000000000003</v>
       </c>
     </row>
@@ -1529,27 +1674,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Consumer Durables</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>1.06</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>1.16</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>1.62</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>-0.09999999999999987</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>-0.5600000000000001</v>
       </c>
     </row>
@@ -1566,27 +1716,32 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Industrial Products</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>Adding</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>0.72</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>0.7</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>0.8</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>0.02000000000000002</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>-0.08000000000000007</v>
       </c>
     </row>
@@ -1603,27 +1758,32 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Consumer Durables</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>0.57</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>0.63</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>0.67</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>-0.06000000000000005</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>-0.1000000000000001</v>
       </c>
     </row>
@@ -1640,27 +1800,32 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Industrial Products</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>Adding</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>0.5600000000000001</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>0.54</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>0.64</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>0.02000000000000002</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>-0.07999999999999996</v>
       </c>
     </row>
@@ -1677,27 +1842,32 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Industrial Products</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>0.46</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>0.48</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>0.52</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>-0.01999999999999996</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>-0.06</v>
       </c>
     </row>
@@ -1714,27 +1884,32 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Industrial Products</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>Reducing Consistently</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>0.39</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>0.4</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>0.46</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>-0.01000000000000001</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>-0.07000000000000001</v>
       </c>
     </row>
@@ -1751,27 +1926,32 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>IT - Software</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>Complete Exit</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>0</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>0.54</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>0.55</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>-0.54</v>
       </c>
-      <c r="I36" t="n">
+      <c r="J36" t="n">
         <v>-0.55</v>
       </c>
     </row>
@@ -1788,27 +1968,32 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Capital Markets</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>Complete Exit</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>0</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>2.49</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>2.27</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>-2.49</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
         <v>-2.27</v>
       </c>
     </row>
@@ -1825,27 +2010,32 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Invesco India Business Cycle Fund</t>
+          <t>Beverages</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
+          <t>Invesco India Business Cycle Fund</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
           <t>Complete Exit</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>0</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>1.59</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>1.73</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>-1.59</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>-1.73</v>
       </c>
     </row>

</xml_diff>